<commit_message>
before frigate, air units done
</commit_message>
<xml_diff>
--- a/SeaWar info/تجهیزات فراوان.xlsx
+++ b/SeaWar info/تجهیزات فراوان.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F864FE2E-2CC8-464B-AC54-2E8651781D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,6 +158,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -204,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +241,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,6 +293,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,32 +485,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="26.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="42.33203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="42.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -489,7 +527,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -530,7 +568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -571,7 +609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -610,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -649,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -688,7 +726,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -727,7 +765,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -766,7 +804,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -805,7 +843,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -844,7 +882,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -883,7 +921,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -922,7 +960,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -961,7 +999,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1000,7 +1038,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1039,7 +1077,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1078,7 +1116,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1117,7 +1155,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1156,7 +1194,7 @@
         <v>9700</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1195,7 +1233,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1234,7 +1272,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1273,7 +1311,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1312,7 +1350,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
@@ -1351,7 +1389,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1368,7 +1406,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1409,7 +1447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -1450,7 +1488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -1491,7 +1529,7 @@
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -1532,7 +1570,7 @@
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>4</v>
       </c>
@@ -1573,7 +1611,7 @@
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>5</v>
       </c>
@@ -1614,7 +1652,7 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>6</v>
       </c>
@@ -1655,7 +1693,7 @@
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>7</v>
       </c>
@@ -1696,7 +1734,7 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>8</v>
       </c>
@@ -1737,7 +1775,7 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -1778,7 +1816,7 @@
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>10</v>
       </c>
@@ -1819,7 +1857,7 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>11</v>
       </c>
@@ -1860,7 +1898,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>12</v>
       </c>
@@ -1901,7 +1939,7 @@
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>13</v>
       </c>
@@ -1942,7 +1980,7 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>14</v>
       </c>
@@ -1983,7 +2021,7 @@
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>15</v>
       </c>
@@ -2024,7 +2062,7 @@
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>16</v>
       </c>
@@ -2065,7 +2103,7 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>17</v>
       </c>
@@ -2106,7 +2144,7 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>18</v>
       </c>
@@ -2147,7 +2185,7 @@
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>19</v>
       </c>
@@ -2188,7 +2226,7 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>20</v>
       </c>
@@ -2229,7 +2267,7 @@
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>21</v>
       </c>
@@ -2270,7 +2308,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
@@ -2287,7 +2325,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>6</v>
       </c>
@@ -2328,7 +2366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>1</v>
       </c>
@@ -2369,7 +2407,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2</v>
       </c>
@@ -2408,7 +2446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>3</v>
       </c>
@@ -2447,7 +2485,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>4</v>
       </c>
@@ -2486,7 +2524,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>5</v>
       </c>
@@ -2525,7 +2563,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>6</v>
       </c>
@@ -2564,7 +2602,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>7</v>
       </c>
@@ -2603,7 +2641,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>8</v>
       </c>
@@ -2642,7 +2680,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>9</v>
       </c>
@@ -2681,7 +2719,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>10</v>
       </c>
@@ -2720,7 +2758,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>11</v>
       </c>
@@ -2759,7 +2797,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>12</v>
       </c>
@@ -2798,7 +2836,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>13</v>
       </c>
@@ -2837,7 +2875,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>14</v>
       </c>
@@ -2876,7 +2914,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>15</v>
       </c>
@@ -2915,7 +2953,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>16</v>
       </c>
@@ -2954,7 +2992,7 @@
         <v>9700</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>17</v>
       </c>
@@ -2993,7 +3031,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>18</v>
       </c>
@@ -3032,7 +3070,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>19</v>
       </c>
@@ -3071,7 +3109,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>20</v>
       </c>
@@ -3110,7 +3148,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>21</v>
       </c>
@@ -3149,7 +3187,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>19</v>
       </c>
@@ -3166,7 +3204,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>6</v>
       </c>
@@ -3207,7 +3245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>1</v>
       </c>
@@ -3248,7 +3286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>2</v>
       </c>
@@ -3289,7 +3327,7 @@
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>3</v>
       </c>
@@ -3330,7 +3368,7 @@
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>4</v>
       </c>
@@ -3371,7 +3409,7 @@
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>5</v>
       </c>
@@ -3412,7 +3450,7 @@
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>6</v>
       </c>
@@ -3453,7 +3491,7 @@
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>7</v>
       </c>
@@ -3494,7 +3532,7 @@
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>8</v>
       </c>
@@ -3535,7 +3573,7 @@
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>9</v>
       </c>
@@ -3576,7 +3614,7 @@
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>10</v>
       </c>
@@ -3617,7 +3655,7 @@
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>11</v>
       </c>
@@ -3658,7 +3696,7 @@
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>12</v>
       </c>
@@ -3699,7 +3737,7 @@
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>13</v>
       </c>
@@ -3740,7 +3778,7 @@
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>14</v>
       </c>
@@ -3781,7 +3819,7 @@
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>15</v>
       </c>
@@ -3822,7 +3860,7 @@
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>16</v>
       </c>
@@ -3863,7 +3901,7 @@
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>17</v>
       </c>
@@ -3904,7 +3942,7 @@
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>18</v>
       </c>
@@ -3945,7 +3983,7 @@
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>19</v>
       </c>
@@ -3986,7 +4024,7 @@
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>20</v>
       </c>
@@ -4027,7 +4065,7 @@
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>21</v>
       </c>
@@ -4068,7 +4106,7 @@
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>22</v>
       </c>
@@ -4085,7 +4123,7 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>6</v>
       </c>
@@ -4126,7 +4164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>1</v>
       </c>
@@ -4167,7 +4205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>2</v>
       </c>
@@ -4208,7 +4246,7 @@
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>3</v>
       </c>
@@ -4249,7 +4287,7 @@
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>4</v>
       </c>
@@ -4290,7 +4328,7 @@
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>5</v>
       </c>
@@ -4331,7 +4369,7 @@
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>6</v>
       </c>
@@ -4372,7 +4410,7 @@
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>7</v>
       </c>
@@ -4413,7 +4451,7 @@
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>8</v>
       </c>
@@ -4454,7 +4492,7 @@
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>9</v>
       </c>
@@ -4495,7 +4533,7 @@
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>10</v>
       </c>
@@ -4536,7 +4574,7 @@
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>11</v>
       </c>
@@ -4577,7 +4615,7 @@
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>12</v>
       </c>
@@ -4618,7 +4656,7 @@
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>13</v>
       </c>
@@ -4659,7 +4697,7 @@
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>14</v>
       </c>
@@ -4700,7 +4738,7 @@
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>15</v>
       </c>
@@ -4741,7 +4779,7 @@
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>16</v>
       </c>
@@ -4782,7 +4820,7 @@
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>17</v>
       </c>
@@ -4823,7 +4861,7 @@
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>18</v>
       </c>
@@ -4864,7 +4902,7 @@
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>19</v>
       </c>
@@ -4905,7 +4943,7 @@
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>20</v>
       </c>
@@ -4946,7 +4984,7 @@
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>21</v>
       </c>
@@ -5001,24 +5039,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>